<commit_message>
fix: add new field encounter-id in screening observation,update documentaion.md,json spec,csv files  #652
</commit_message>
<xml_diff>
--- a/support/specifications/flat-file/nyher-fhir-ig-example/Winter-24-CSV.xlsx
+++ b/support/specifications/flat-file/nyher-fhir-ig-example/Winter-24-CSV.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28409"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B84FAF5-077D-404C-8EBB-CCC5E3E78D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{372AB003-6A0B-4EFD-8FF1-EF70A1BCF6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demographic Data" sheetId="1" r:id="rId1"/>
     <sheet name="QE Admin Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Screening Observation" sheetId="3" r:id="rId3"/>
-    <sheet name="Screening Details" sheetId="9" r:id="rId4"/>
+    <sheet name="Screening Profile" sheetId="9" r:id="rId3"/>
+    <sheet name="Screening Observation" sheetId="3" r:id="rId4"/>
     <sheet name="Change Log" sheetId="4" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Change Log'!$A$1:$N$97</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -490,7 +493,144 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={72896948-814B-4594-B32F-3DEFD4CEBA1B}</author>
+    <author>tc={AB8D73DF-236D-457D-87B0-F8D41364C443}</author>
+    <author>tc={AE35D772-A976-4C9F-B0FF-7C45AA1191A3}</author>
+    <author>tc={804B06AA-065C-4091-83E0-ACEE1A81B407}</author>
+    <author>tc={536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}</author>
+    <author>tc={62B258D0-7A4F-4FEB-9191-89D31F562217}</author>
+    <author>tc={3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}</author>
+    <author>tc={681C1D15-B369-4B3C-919A-2F0B2215C813}</author>
+    <author>tc={486CC9F5-0999-4F96-9923-5B32950F15F6}</author>
+    <author>tc={D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}</author>
+    <author>tc={4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}</author>
+    <author>tc={7FA6E572-1D70-4E8A-926E-72DE9823A3CA}</author>
+    <author>tc={205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}</author>
+    <author>tc={1A4E7674-30A3-4079-AD5C-85FD44338686}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{72896948-814B-4594-B32F-3DEFD4CEBA1B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    PAT_MRN_ID changed to PATIENT_MR_ID_VALUE. 
+This id will be found in the FHIR Patient resource -&gt;identifier-&gt;value where Patient resource -&gt;identifier-&gt;type-&gt; code is MR</t>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{AB8D73DF-236D-457D-87B0-F8D41364C443}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;id</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{AE35D772-A976-4C9F-B0FF-7C45AA1191A3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;class-&gt; code</t>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{804B06AA-065C-4091-83E0-ACEE1A81B407}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;status</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; code</t>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{62B258D0-7A4F-4FEB-9191-89D31F562217}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;type-&gt; text</t>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; system</t>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{681C1D15-B369-4B3C-919A-2F0B2215C813}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This time will be found in the FHIR Encounter resource -&gt;meta -&gt; lastUpdated</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{486CC9F5-0999-4F96-9923-5B32950F15F6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the FHIR Consent resource -&gt;meta -&gt; lastUpdated</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the FHIR Consent resource -&gt;dateTime</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the FHIR Consent resource -&gt;policy-&gt; authority </t>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{7FA6E572-1D70-4E8A-926E-72DE9823A3CA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the FHIR Consent resource -&gt;provision-&gt; type</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the  FHIR Observation resource -&gt;meta -&gt; lastUpdated</t>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{1A4E7674-30A3-4079-AD5C-85FD44338686}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This data will be found in the  FHIR Observation resource -&gt;status</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={AA13E25F-FE68-4156-9DEB-4BCE28A9048C}</author>
+    <author>tc={04DE7DCA-F748-4589-B2AB-4B3568CDF66F}</author>
     <author>tc={8A263F6E-AEAA-4CFA-AAAD-27134A08649F}</author>
     <author>tc={349F7E7F-3512-43A9-881A-6C897DAA5E48}</author>
     <author>tc={BEA77AA8-6911-4D0E-BA59-4AF96FC0F5C3}</author>
@@ -518,7 +658,15 @@
 This id will be found in the FHIR Patient resource -&gt;identifier-&gt;value where Patient resource -&gt;identifier-&gt;type-&gt; code is MR</t>
       </text>
     </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{8A263F6E-AEAA-4CFA-AAAD-27134A08649F}">
+    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{04DE7DCA-F748-4589-B2AB-4B3568CDF66F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This value can be found in the FHIR Encounter resource -&gt;id</t>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{8A263F6E-AEAA-4CFA-AAAD-27134A08649F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -526,7 +674,7 @@
     This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is a grouper </t>
       </text>
     </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{349F7E7F-3512-43A9-881A-6C897DAA5E48}">
+    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{349F7E7F-3512-43A9-881A-6C897DAA5E48}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -534,7 +682,7 @@
     This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is a grouper </t>
       </text>
     </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{BEA77AA8-6911-4D0E-BA59-4AF96FC0F5C3}">
+    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{BEA77AA8-6911-4D0E-BA59-4AF96FC0F5C3}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -542,7 +690,7 @@
     This data will be found in the FHIR Observation resource -&gt; effectiveDateTime</t>
       </text>
     </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{F014D3FF-B0BC-4BA1-8AF2-613B494BE08F}">
+    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{F014D3FF-B0BC-4BA1-8AF2-613B494BE08F}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -550,7 +698,7 @@
     This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is not a grouper </t>
       </text>
     </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{4B928C03-4EF4-497D-814C-FC9F483A5B10}">
+    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{4B928C03-4EF4-497D-814C-FC9F483A5B10}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -558,7 +706,7 @@
     This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is not a grouper </t>
       </text>
     </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{74CF8398-8030-4A1C-A795-9852ECDC31A6}">
+    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{74CF8398-8030-4A1C-A795-9852ECDC31A6}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -566,7 +714,7 @@
     This data will be found in the FHIR Observation resource -&gt;code-&gt; text where the observation is not a grouper </t>
       </text>
     </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{4407F58D-3F19-4F13-B62F-9F0B6D5F561F}">
+    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{4407F58D-3F19-4F13-B62F-9F0B6D5F561F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -574,7 +722,7 @@
     This data will be found in the FHIR Observation resource -&gt;category-&gt; text where the category is SDOH and the SDOH category is SDOH Category Unspecified</t>
       </text>
     </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{A958652F-7E6D-4528-AD64-EC68E3B0AFC8}">
+    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{A958652F-7E6D-4528-AD64-EC68E3B0AFC8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -582,7 +730,7 @@
     This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SDOH </t>
       </text>
     </comment>
-    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{CB537BA9-625D-4386-86A0-060B722D2075}">
+    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{CB537BA9-625D-4386-86A0-060B722D2075}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -590,7 +738,7 @@
     This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is SDOH </t>
       </text>
     </comment>
-    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{AC728550-8F53-4B6C-85A8-DB8CFBEFF7F1}">
+    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{AC728550-8F53-4B6C-85A8-DB8CFBEFF7F1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -598,7 +746,7 @@
     This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SNOMED</t>
       </text>
     </comment>
-    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{1DC423B6-3560-466F-B8E0-1431647C66FD}">
+    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{1DC423B6-3560-466F-B8E0-1431647C66FD}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -606,7 +754,7 @@
     This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is Snomed</t>
       </text>
     </comment>
-    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{34244F04-54B6-41D6-AF91-9EB079B0A4E7}">
+    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{34244F04-54B6-41D6-AF91-9EB079B0A4E7}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -614,7 +762,7 @@
     This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; code. </t>
       </text>
     </comment>
-    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{20679167-3EA0-43E7-B53A-F8FAB7648DB8}">
+    <comment ref="O1" authorId="14" shapeId="0" xr:uid="{20679167-3EA0-43E7-B53A-F8FAB7648DB8}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -622,7 +770,7 @@
     This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; display. </t>
       </text>
     </comment>
-    <comment ref="O1" authorId="14" shapeId="0" xr:uid="{6CA91F97-61DA-4680-8A35-029D10FD956E}">
+    <comment ref="P1" authorId="15" shapeId="0" xr:uid="{6CA91F97-61DA-4680-8A35-029D10FD956E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -630,7 +778,7 @@
     This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; code. </t>
       </text>
     </comment>
-    <comment ref="P1" authorId="15" shapeId="0" xr:uid="{47214620-2989-43D4-8755-5B653BA0351D}">
+    <comment ref="Q1" authorId="16" shapeId="0" xr:uid="{47214620-2989-43D4-8755-5B653BA0351D}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -638,148 +786,12 @@
     This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; display. </t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="16" shapeId="0" xr:uid="{43671D0C-A6DE-4288-830A-962F5698A778}">
+    <comment ref="R1" authorId="17" shapeId="0" xr:uid="{43671D0C-A6DE-4288-830A-962F5698A778}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; text </t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={72896948-814B-4594-B32F-3DEFD4CEBA1B}</author>
-    <author>tc={AB8D73DF-236D-457D-87B0-F8D41364C443}</author>
-    <author>tc={AE35D772-A976-4C9F-B0FF-7C45AA1191A3}</author>
-    <author>tc={804B06AA-065C-4091-83E0-ACEE1A81B407}</author>
-    <author>tc={536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}</author>
-    <author>tc={62B258D0-7A4F-4FEB-9191-89D31F562217}</author>
-    <author>tc={3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}</author>
-    <author>tc={681C1D15-B369-4B3C-919A-2F0B2215C813}</author>
-    <author>tc={486CC9F5-0999-4F96-9923-5B32950F15F6}</author>
-    <author>tc={D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}</author>
-    <author>tc={4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}</author>
-    <author>tc={7FA6E572-1D70-4E8A-926E-72DE9823A3CA}</author>
-    <author>tc={205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}</author>
-    <author>tc={1A4E7674-30A3-4079-AD5C-85FD44338686}</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{72896948-814B-4594-B32F-3DEFD4CEBA1B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    PAT_MRN_ID changed to PATIENT_MR_ID_VALUE. 
-This id will be found in the FHIR Patient resource -&gt;identifier-&gt;value where Patient resource -&gt;identifier-&gt;type-&gt; code is MR</t>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="1" shapeId="0" xr:uid="{AB8D73DF-236D-457D-87B0-F8D41364C443}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;id</t>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="2" shapeId="0" xr:uid="{AE35D772-A976-4C9F-B0FF-7C45AA1191A3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;class-&gt; code</t>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="3" shapeId="0" xr:uid="{804B06AA-065C-4091-83E0-ACEE1A81B407}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;status</t>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="4" shapeId="0" xr:uid="{536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; code</t>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="5" shapeId="0" xr:uid="{62B258D0-7A4F-4FEB-9191-89D31F562217}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;type-&gt; text</t>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="6" shapeId="0" xr:uid="{3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; system</t>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="7" shapeId="0" xr:uid="{681C1D15-B369-4B3C-919A-2F0B2215C813}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This time will be found in the FHIR Encounter resource -&gt;meta -&gt; lastUpdated</t>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="8" shapeId="0" xr:uid="{486CC9F5-0999-4F96-9923-5B32950F15F6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the FHIR Consent resource -&gt;meta -&gt; lastUpdated</t>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="9" shapeId="0" xr:uid="{D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the FHIR Consent resource -&gt;dateTime</t>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="10" shapeId="0" xr:uid="{4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}">
-      <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the FHIR Consent resource -&gt;policy-&gt; authority </t>
-      </text>
-    </comment>
-    <comment ref="L1" authorId="11" shapeId="0" xr:uid="{7FA6E572-1D70-4E8A-926E-72DE9823A3CA}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the FHIR Consent resource -&gt;provision-&gt; type</t>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="12" shapeId="0" xr:uid="{205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the  FHIR Observation resource -&gt;meta -&gt; lastUpdated</t>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="13" shapeId="0" xr:uid="{1A4E7674-30A3-4079-AD5C-85FD44338686}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    This data will be found in the  FHIR Observation resource -&gt;status</t>
       </text>
     </comment>
   </commentList>
@@ -787,7 +799,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="325">
   <si>
     <t>PATIENT_MR_ID_VALUE</t>
   </si>
@@ -1071,6 +1083,66 @@
     <t>http://www.scn.ny.gov/</t>
   </si>
   <si>
+    <t>ENCOUNTER_ID</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_CLASS_CODE</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_TYPE_CODE</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_TYPE_CODE_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_TYPE_CODE_SYSTEM</t>
+  </si>
+  <si>
+    <t>ENCOUNTER_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>CONSENT_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>CONSENT_DATE_TIME</t>
+  </si>
+  <si>
+    <t>CONSENT_POLICY_AUTHORITY</t>
+  </si>
+  <si>
+    <t>CONSENT_PROVISION_TYPE</t>
+  </si>
+  <si>
+    <t>SCREENING_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>SCREENING_STATUS_CODE</t>
+  </si>
+  <si>
+    <t>EncounterExample</t>
+  </si>
+  <si>
+    <t>FLD</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>Direct questioning (procedure)</t>
+  </si>
+  <si>
+    <t>urn:uuid:d1eaac1a-22b7-4bb6-9c62-cc95d6fdf1a5</t>
+  </si>
+  <si>
+    <t>permit</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
     <t>SCREENING_CODE</t>
   </si>
   <si>
@@ -1566,66 +1638,6 @@
     <t>Because of a physical, mental, or emotional condition, do you have difficulty doing errands alone such as visiting a physician's office or shopping</t>
   </si>
   <si>
-    <t>ENCOUNTER_ID</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_CLASS_CODE</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_STATUS_CODE</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_TYPE_CODE</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_TYPE_CODE_DESCRIPTION</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_TYPE_CODE_SYSTEM</t>
-  </si>
-  <si>
-    <t>ENCOUNTER_LAST_UPDATED</t>
-  </si>
-  <si>
-    <t>CONSENT_LAST_UPDATED</t>
-  </si>
-  <si>
-    <t>CONSENT_DATE_TIME</t>
-  </si>
-  <si>
-    <t>CONSENT_POLICY_AUTHORITY</t>
-  </si>
-  <si>
-    <t>CONSENT_PROVISION_TYPE</t>
-  </si>
-  <si>
-    <t>SCREENING_LAST_UPDATED</t>
-  </si>
-  <si>
-    <t>SCREENING_STATUS_CODE</t>
-  </si>
-  <si>
-    <t>EncounterExample</t>
-  </si>
-  <si>
-    <t>FLD</t>
-  </si>
-  <si>
-    <t>finished</t>
-  </si>
-  <si>
-    <t>Direct questioning (procedure)</t>
-  </si>
-  <si>
-    <t>urn:uuid:d1eaac1a-22b7-4bb6-9c62-cc95d6fdf1a5</t>
-  </si>
-  <si>
-    <t>permit</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
     <t>This sheet explains all the diffeence between trhe business logic and schema described in the original excel docuemt at url and SHIN-NY IG version v1.0.0. Needs to be updated.</t>
   </si>
   <si>
@@ -1755,22 +1767,13 @@
     <t>0..*</t>
   </si>
   <si>
-    <t>Screening file has been removed and the data from screening is covered under the files Screening Observation, Screening Details</t>
+    <t>Screening file has been removed and the data from screening is covered under the files Screening Observation, Screening Profile</t>
   </si>
   <si>
     <t>Screening Observation</t>
   </si>
   <si>
-    <t>Screening Details</t>
-  </si>
-  <si>
-    <t>Screening Encounter</t>
-  </si>
-  <si>
-    <t>Screening Consent</t>
-  </si>
-  <si>
-    <t>Screening Resources</t>
+    <t>Screening Profile</t>
   </si>
 </sst>
 </file>
@@ -1904,7 +1907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1934,6 +1937,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1943,11 +1949,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2446,105 +2447,108 @@
 
 <file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2024-11-12T16:16:39.32" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AA13E25F-FE68-4156-9DEB-4BCE28A9048C}">
+  <threadedComment ref="A1" dT="2024-11-12T16:16:39.32" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{72896948-814B-4594-B32F-3DEFD4CEBA1B}">
     <text>PAT_MRN_ID changed to PATIENT_MR_ID_VALUE. 
 This id will be found in the FHIR Patient resource -&gt;identifier-&gt;value where Patient resource -&gt;identifier-&gt;type-&gt; code is MR</text>
   </threadedComment>
-  <threadedComment ref="B1" dT="2024-11-26T17:13:40.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{8A263F6E-AEAA-4CFA-AAAD-27134A08649F}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is a grouper </text>
-  </threadedComment>
-  <threadedComment ref="C1" dT="2024-11-26T17:14:01.87" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{349F7E7F-3512-43A9-881A-6C897DAA5E48}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is a grouper </text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2024-11-26T17:17:49.79" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{BEA77AA8-6911-4D0E-BA59-4AF96FC0F5C3}">
-    <text>This data will be found in the FHIR Observation resource -&gt; effectiveDateTime</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2024-11-26T17:21:17.73" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{F014D3FF-B0BC-4BA1-8AF2-613B494BE08F}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is not a grouper </text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2024-11-26T17:21:30.01" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4B928C03-4EF4-497D-814C-FC9F483A5B10}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is not a grouper </text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2024-11-26T17:21:59.98" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{74CF8398-8030-4A1C-A795-9852ECDC31A6}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt; text where the observation is not a grouper </text>
-  </threadedComment>
-  <threadedComment ref="H1" dT="2024-11-27T04:09:17.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4407F58D-3F19-4F13-B62F-9F0B6D5F561F}">
-    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; text where the category is SDOH and the SDOH category is SDOH Category Unspecified</text>
-  </threadedComment>
-  <threadedComment ref="I1" dT="2024-11-27T04:09:55.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{A958652F-7E6D-4528-AD64-EC68E3B0AFC8}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SDOH </text>
-  </threadedComment>
-  <threadedComment ref="J1" dT="2024-11-27T04:10:48.91" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{CB537BA9-625D-4386-86A0-060B722D2075}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is SDOH </text>
-  </threadedComment>
-  <threadedComment ref="K1" dT="2024-11-27T04:11:33.02" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AC728550-8F53-4B6C-85A8-DB8CFBEFF7F1}">
-    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SNOMED</text>
-  </threadedComment>
-  <threadedComment ref="L1" dT="2024-11-27T04:12:02.38" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{1DC423B6-3560-466F-B8E0-1431647C66FD}">
-    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is Snomed</text>
-  </threadedComment>
-  <threadedComment ref="M1" dT="2024-11-27T04:13:42.78" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{34244F04-54B6-41D6-AF91-9EB079B0A4E7}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; code. </text>
-  </threadedComment>
-  <threadedComment ref="N1" dT="2024-11-27T04:13:56.21" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{20679167-3EA0-43E7-B53A-F8FAB7648DB8}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; display. </text>
-  </threadedComment>
-  <threadedComment ref="O1" dT="2024-11-27T12:45:36.80" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{6CA91F97-61DA-4680-8A35-029D10FD956E}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; code. </text>
-  </threadedComment>
-  <threadedComment ref="P1" dT="2024-11-27T12:45:53.61" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{47214620-2989-43D4-8755-5B653BA0351D}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; display. </text>
-  </threadedComment>
-  <threadedComment ref="Q1" dT="2024-11-27T12:45:53.61" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{43671D0C-A6DE-4288-830A-962F5698A778}">
-    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; text </text>
+  <threadedComment ref="B1" dT="2024-11-26T16:54:13.96" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AB8D73DF-236D-457D-87B0-F8D41364C443}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;id</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2024-11-26T16:54:38.88" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AE35D772-A976-4C9F-B0FF-7C45AA1191A3}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;class-&gt; code</text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2024-11-26T16:56:39.49" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{804B06AA-065C-4091-83E0-ACEE1A81B407}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;status</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2024-11-26T16:58:06.67" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; code</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2024-11-26T16:58:32.95" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{62B258D0-7A4F-4FEB-9191-89D31F562217}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; text</text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2024-11-26T16:58:54.34" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}">
+    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; system</text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2024-11-13T08:20:35.99" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{681C1D15-B369-4B3C-919A-2F0B2215C813}">
+    <text>This time will be found in the FHIR Encounter resource -&gt;meta -&gt; lastUpdated</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2024-11-27T04:34:23.34" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{486CC9F5-0999-4F96-9923-5B32950F15F6}">
+    <text>This data will be found in the FHIR Consent resource -&gt;meta -&gt; lastUpdated</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2024-11-27T04:44:44.92" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}">
+    <text>This data will be found in the FHIR Consent resource -&gt;dateTime</text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2024-11-27T04:43:14.86" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}">
+    <text xml:space="preserve">This data will be found in the FHIR Consent resource -&gt;policy-&gt; authority </text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2024-11-27T04:45:09.38" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{7FA6E572-1D70-4E8A-926E-72DE9823A3CA}">
+    <text>This data will be found in the FHIR Consent resource -&gt;provision-&gt; type</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2024-11-27T04:57:51.11" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}">
+    <text>This data will be found in the  FHIR Observation resource -&gt;meta -&gt; lastUpdated</text>
+  </threadedComment>
+  <threadedComment ref="N1" dT="2024-11-13T09:10:26.90" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{1A4E7674-30A3-4079-AD5C-85FD44338686}">
+    <text>This data will be found in the  FHIR Observation resource -&gt;status</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A1" dT="2024-11-12T16:16:39.32" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{72896948-814B-4594-B32F-3DEFD4CEBA1B}">
+  <threadedComment ref="A1" dT="2024-11-12T16:16:39.32" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AA13E25F-FE68-4156-9DEB-4BCE28A9048C}">
     <text>PAT_MRN_ID changed to PATIENT_MR_ID_VALUE. 
 This id will be found in the FHIR Patient resource -&gt;identifier-&gt;value where Patient resource -&gt;identifier-&gt;type-&gt; code is MR</text>
   </threadedComment>
-  <threadedComment ref="B1" dT="2024-11-26T16:54:13.96" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AB8D73DF-236D-457D-87B0-F8D41364C443}">
+  <threadedComment ref="B1" dT="2024-11-26T16:54:13.96" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{04DE7DCA-F748-4589-B2AB-4B3568CDF66F}">
     <text>This value can be found in the FHIR Encounter resource -&gt;id</text>
   </threadedComment>
-  <threadedComment ref="C1" dT="2024-11-26T16:54:38.88" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AE35D772-A976-4C9F-B0FF-7C45AA1191A3}">
-    <text>This value can be found in the FHIR Encounter resource -&gt;class-&gt; code</text>
-  </threadedComment>
-  <threadedComment ref="D1" dT="2024-11-26T16:56:39.49" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{804B06AA-065C-4091-83E0-ACEE1A81B407}">
-    <text>This value can be found in the FHIR Encounter resource -&gt;status</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2024-11-26T16:58:06.67" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{536C0056-6E9A-49E5-8BD9-CAF00DCBCA85}">
-    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; code</text>
-  </threadedComment>
-  <threadedComment ref="F1" dT="2024-11-26T16:58:32.95" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{62B258D0-7A4F-4FEB-9191-89D31F562217}">
-    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; text</text>
-  </threadedComment>
-  <threadedComment ref="G1" dT="2024-11-26T16:58:54.34" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{3C505D42-CBBD-4A9C-9FC4-F0DBC06284A3}">
-    <text>This value can be found in the FHIR Encounter resource -&gt;type-&gt; coding-&gt; system</text>
-  </threadedComment>
-  <threadedComment ref="H1" dT="2024-11-13T08:20:35.99" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{681C1D15-B369-4B3C-919A-2F0B2215C813}">
-    <text>This time will be found in the FHIR Encounter resource -&gt;meta -&gt; lastUpdated</text>
-  </threadedComment>
-  <threadedComment ref="I1" dT="2024-11-27T04:34:23.34" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{486CC9F5-0999-4F96-9923-5B32950F15F6}">
-    <text>This data will be found in the FHIR Consent resource -&gt;meta -&gt; lastUpdated</text>
-  </threadedComment>
-  <threadedComment ref="J1" dT="2024-11-27T04:44:44.92" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{D9E1D673-F98D-47F0-B28B-7E8DD1359EA5}">
-    <text>This data will be found in the FHIR Consent resource -&gt;dateTime</text>
-  </threadedComment>
-  <threadedComment ref="K1" dT="2024-11-27T04:43:14.86" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4D2BC01E-23F0-4D28-A28A-6E193E7A9B3C}">
-    <text xml:space="preserve">This data will be found in the FHIR Consent resource -&gt;policy-&gt; authority </text>
-  </threadedComment>
-  <threadedComment ref="L1" dT="2024-11-27T04:45:09.38" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{7FA6E572-1D70-4E8A-926E-72DE9823A3CA}">
-    <text>This data will be found in the FHIR Consent resource -&gt;provision-&gt; type</text>
-  </threadedComment>
-  <threadedComment ref="M1" dT="2024-11-27T04:57:51.11" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{205D5BEF-D18E-4444-80F7-B45EEC2E1BE9}">
-    <text>This data will be found in the  FHIR Observation resource -&gt;meta -&gt; lastUpdated</text>
-  </threadedComment>
-  <threadedComment ref="N1" dT="2024-11-13T09:10:26.90" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{1A4E7674-30A3-4079-AD5C-85FD44338686}">
-    <text>This data will be found in the  FHIR Observation resource -&gt;status</text>
+  <threadedComment ref="C1" dT="2024-11-26T17:13:40.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{8A263F6E-AEAA-4CFA-AAAD-27134A08649F}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is a grouper </text>
+  </threadedComment>
+  <threadedComment ref="D1" dT="2024-11-26T17:14:01.87" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{349F7E7F-3512-43A9-881A-6C897DAA5E48}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is a grouper </text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2024-11-26T17:17:49.79" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{BEA77AA8-6911-4D0E-BA59-4AF96FC0F5C3}">
+    <text>This data will be found in the FHIR Observation resource -&gt; effectiveDateTime</text>
+  </threadedComment>
+  <threadedComment ref="F1" dT="2024-11-26T17:21:17.73" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{F014D3FF-B0BC-4BA1-8AF2-613B494BE08F}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; code where the observation is not a grouper </text>
+  </threadedComment>
+  <threadedComment ref="G1" dT="2024-11-26T17:21:30.01" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4B928C03-4EF4-497D-814C-FC9F483A5B10}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt;coding -&gt; display where the observation is not a grouper </text>
+  </threadedComment>
+  <threadedComment ref="H1" dT="2024-11-26T17:21:59.98" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{74CF8398-8030-4A1C-A795-9852ECDC31A6}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;code-&gt; text where the observation is not a grouper </text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2024-11-27T04:09:17.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{4407F58D-3F19-4F13-B62F-9F0B6D5F561F}">
+    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; text where the category is SDOH and the SDOH category is SDOH Category Unspecified</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2024-11-27T04:09:55.65" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{A958652F-7E6D-4528-AD64-EC68E3B0AFC8}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SDOH </text>
+  </threadedComment>
+  <threadedComment ref="K1" dT="2024-11-27T04:10:48.91" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{CB537BA9-625D-4386-86A0-060B722D2075}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is SDOH </text>
+  </threadedComment>
+  <threadedComment ref="L1" dT="2024-11-27T04:11:33.02" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{AC728550-8F53-4B6C-85A8-DB8CFBEFF7F1}">
+    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; code where the category is SNOMED</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2024-11-27T04:12:02.38" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{1DC423B6-3560-466F-B8E0-1431647C66FD}">
+    <text>This data will be found in the FHIR Observation resource -&gt;category-&gt; coding-&gt; display where the category is Snomed</text>
+  </threadedComment>
+  <threadedComment ref="N1" dT="2024-11-27T04:13:42.78" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{34244F04-54B6-41D6-AF91-9EB079B0A4E7}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; code. </text>
+  </threadedComment>
+  <threadedComment ref="O1" dT="2024-11-27T04:13:56.21" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{20679167-3EA0-43E7-B53A-F8FAB7648DB8}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;valueCodeableConcept-&gt; coding-&gt; display. </text>
+  </threadedComment>
+  <threadedComment ref="P1" dT="2024-11-27T12:45:36.80" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{6CA91F97-61DA-4680-8A35-029D10FD956E}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; code. </text>
+  </threadedComment>
+  <threadedComment ref="Q1" dT="2024-11-27T12:45:53.61" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{47214620-2989-43D4-8755-5B653BA0351D}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; coding-&gt; display. </text>
+  </threadedComment>
+  <threadedComment ref="R1" dT="2024-11-27T12:45:53.61" personId="{ADC9734B-05B3-4808-97FB-8C215A4A250A}" id="{43671D0C-A6DE-4288-830A-962F5698A778}">
+    <text xml:space="preserve">This data will be found in the FHIR Observation resource -&gt;dataAbsentReason-&gt; text </text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -2553,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2848,8 +2852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0E656CF-E116-470E-A3B2-FBFB1DA8B1CF}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2879,7 +2883,7 @@
       <c r="C1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -2953,7 +2957,7 @@
       <c r="M2" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="21" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2967,1157 +2971,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCE62ED-6F52-49FE-89FA-F3C6891E8BA9}">
-  <dimension ref="A1:Q31"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="127.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="196" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="46.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="31.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G2" t="s">
-        <v>115</v>
-      </c>
-      <c r="I2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M2" t="s">
-        <v>118</v>
-      </c>
-      <c r="N2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I3" t="s">
-        <v>123</v>
-      </c>
-      <c r="J3" t="s">
-        <v>124</v>
-      </c>
-      <c r="M3" t="s">
-        <v>125</v>
-      </c>
-      <c r="N3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" t="s">
-        <v>127</v>
-      </c>
-      <c r="F4" t="s">
-        <v>128</v>
-      </c>
-      <c r="G4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I4" t="s">
-        <v>130</v>
-      </c>
-      <c r="J4" t="s">
-        <v>131</v>
-      </c>
-      <c r="M4" t="s">
-        <v>132</v>
-      </c>
-      <c r="N4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J5" t="s">
-        <v>131</v>
-      </c>
-      <c r="M5" t="s">
-        <v>132</v>
-      </c>
-      <c r="N5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F6" t="s">
-        <v>138</v>
-      </c>
-      <c r="G6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I6" t="s">
-        <v>140</v>
-      </c>
-      <c r="J6" t="s">
-        <v>141</v>
-      </c>
-      <c r="M6" t="s">
-        <v>142</v>
-      </c>
-      <c r="N6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" t="s">
-        <v>147</v>
-      </c>
-      <c r="J7" t="s">
-        <v>148</v>
-      </c>
-      <c r="M7" t="s">
-        <v>142</v>
-      </c>
-      <c r="N7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" t="s">
-        <v>149</v>
-      </c>
-      <c r="F8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" t="s">
-        <v>151</v>
-      </c>
-      <c r="H8" t="s">
-        <v>152</v>
-      </c>
-      <c r="I8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J8" t="s">
-        <v>154</v>
-      </c>
-      <c r="M8" t="s">
-        <v>155</v>
-      </c>
-      <c r="N8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G9" t="s">
-        <v>159</v>
-      </c>
-      <c r="H9" t="s">
-        <v>152</v>
-      </c>
-      <c r="I9" t="s">
-        <v>153</v>
-      </c>
-      <c r="J9" t="s">
-        <v>154</v>
-      </c>
-      <c r="M9" t="s">
-        <v>155</v>
-      </c>
-      <c r="N9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" t="s">
-        <v>111</v>
-      </c>
-      <c r="D10" t="s">
-        <v>112</v>
-      </c>
-      <c r="E10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H10" t="s">
-        <v>152</v>
-      </c>
-      <c r="I10" t="s">
-        <v>153</v>
-      </c>
-      <c r="J10" t="s">
-        <v>154</v>
-      </c>
-      <c r="M10" t="s">
-        <v>155</v>
-      </c>
-      <c r="N10" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D11" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" t="s">
-        <v>163</v>
-      </c>
-      <c r="F11" t="s">
-        <v>164</v>
-      </c>
-      <c r="G11" t="s">
-        <v>165</v>
-      </c>
-      <c r="H11" t="s">
-        <v>152</v>
-      </c>
-      <c r="I11" t="s">
-        <v>153</v>
-      </c>
-      <c r="J11" t="s">
-        <v>154</v>
-      </c>
-      <c r="M11" t="s">
-        <v>155</v>
-      </c>
-      <c r="N11" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
-      <c r="A12" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B12" t="s">
-        <v>110</v>
-      </c>
-      <c r="C12" t="s">
-        <v>111</v>
-      </c>
-      <c r="D12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" t="s">
-        <v>166</v>
-      </c>
-      <c r="F12" t="s">
-        <v>167</v>
-      </c>
-      <c r="G12" t="s">
-        <v>168</v>
-      </c>
-      <c r="H12" t="s">
-        <v>152</v>
-      </c>
-      <c r="I12" t="s">
-        <v>153</v>
-      </c>
-      <c r="J12" t="s">
-        <v>154</v>
-      </c>
-      <c r="N12" s="10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
-      <c r="A13" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B13" t="s">
-        <v>169</v>
-      </c>
-      <c r="C13" t="s">
-        <v>170</v>
-      </c>
-      <c r="D13" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>171</v>
-      </c>
-      <c r="F13" t="s">
-        <v>172</v>
-      </c>
-      <c r="G13" t="s">
-        <v>173</v>
-      </c>
-      <c r="I13" t="s">
-        <v>174</v>
-      </c>
-      <c r="J13" t="s">
-        <v>175</v>
-      </c>
-      <c r="M13" t="s">
-        <v>176</v>
-      </c>
-      <c r="N13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
-      <c r="A14" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B14" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" t="s">
-        <v>178</v>
-      </c>
-      <c r="F14" t="s">
-        <v>179</v>
-      </c>
-      <c r="G14" t="s">
-        <v>180</v>
-      </c>
-      <c r="I14" t="s">
-        <v>181</v>
-      </c>
-      <c r="J14" t="s">
-        <v>182</v>
-      </c>
-      <c r="M14" t="s">
-        <v>183</v>
-      </c>
-      <c r="N14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
-      <c r="A15" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C15" t="s">
-        <v>170</v>
-      </c>
-      <c r="D15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" t="s">
-        <v>185</v>
-      </c>
-      <c r="F15" t="s">
-        <v>186</v>
-      </c>
-      <c r="G15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15" t="s">
-        <v>188</v>
-      </c>
-      <c r="J15" t="s">
-        <v>189</v>
-      </c>
-      <c r="M15" t="s">
-        <v>190</v>
-      </c>
-      <c r="N15" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B16" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D16" t="s">
-        <v>112</v>
-      </c>
-      <c r="E16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F16" t="s">
-        <v>193</v>
-      </c>
-      <c r="G16" t="s">
-        <v>194</v>
-      </c>
-      <c r="I16" t="s">
-        <v>188</v>
-      </c>
-      <c r="J16" t="s">
-        <v>189</v>
-      </c>
-      <c r="M16" t="s">
-        <v>155</v>
-      </c>
-      <c r="N16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
-      <c r="A17" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" t="s">
-        <v>197</v>
-      </c>
-      <c r="K17">
-        <v>106133000</v>
-      </c>
-      <c r="L17" t="s">
-        <v>198</v>
-      </c>
-      <c r="M17" t="s">
-        <v>199</v>
-      </c>
-      <c r="N17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B18" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" t="s">
-        <v>112</v>
-      </c>
-      <c r="E18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" t="s">
-        <v>202</v>
-      </c>
-      <c r="G18" t="s">
-        <v>203</v>
-      </c>
-      <c r="K18">
-        <v>365458002</v>
-      </c>
-      <c r="L18" t="s">
-        <v>204</v>
-      </c>
-      <c r="M18" t="s">
-        <v>199</v>
-      </c>
-      <c r="N18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="A19" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" t="s">
-        <v>170</v>
-      </c>
-      <c r="D19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G19" t="s">
-        <v>207</v>
-      </c>
-      <c r="K19">
-        <v>129861002</v>
-      </c>
-      <c r="L19" t="s">
-        <v>208</v>
-      </c>
-      <c r="M19" t="s">
-        <v>209</v>
-      </c>
-      <c r="N19" s="10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B20" t="s">
-        <v>169</v>
-      </c>
-      <c r="C20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D20" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" t="s">
-        <v>210</v>
-      </c>
-      <c r="F20" t="s">
-        <v>211</v>
-      </c>
-      <c r="G20" t="s">
-        <v>212</v>
-      </c>
-      <c r="K20">
-        <v>129861002</v>
-      </c>
-      <c r="L20" t="s">
-        <v>208</v>
-      </c>
-      <c r="M20" t="s">
-        <v>213</v>
-      </c>
-      <c r="N20" s="10">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B21" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" t="s">
-        <v>170</v>
-      </c>
-      <c r="D21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E21" t="s">
-        <v>214</v>
-      </c>
-      <c r="F21" t="s">
-        <v>215</v>
-      </c>
-      <c r="G21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="A22" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B22" t="s">
-        <v>169</v>
-      </c>
-      <c r="C22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D22" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" t="s">
-        <v>217</v>
-      </c>
-      <c r="F22" t="s">
-        <v>218</v>
-      </c>
-      <c r="G22" t="s">
-        <v>219</v>
-      </c>
-      <c r="K22">
-        <v>228273003</v>
-      </c>
-      <c r="L22" t="s">
-        <v>220</v>
-      </c>
-      <c r="M22" t="s">
-        <v>221</v>
-      </c>
-      <c r="N22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="A23" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C23" t="s">
-        <v>170</v>
-      </c>
-      <c r="D23" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" t="s">
-        <v>223</v>
-      </c>
-      <c r="F23" t="s">
-        <v>224</v>
-      </c>
-      <c r="G23" t="s">
-        <v>225</v>
-      </c>
-      <c r="K23">
-        <v>365980008</v>
-      </c>
-      <c r="L23" t="s">
-        <v>226</v>
-      </c>
-      <c r="M23" t="s">
-        <v>221</v>
-      </c>
-      <c r="N23" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="A24" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B24" t="s">
-        <v>169</v>
-      </c>
-      <c r="C24" t="s">
-        <v>170</v>
-      </c>
-      <c r="D24" t="s">
-        <v>112</v>
-      </c>
-      <c r="E24" t="s">
-        <v>227</v>
-      </c>
-      <c r="F24" t="s">
-        <v>228</v>
-      </c>
-      <c r="G24" t="s">
-        <v>229</v>
-      </c>
-      <c r="K24">
-        <v>409069009</v>
-      </c>
-      <c r="L24" t="s">
-        <v>230</v>
-      </c>
-      <c r="M24" t="s">
-        <v>221</v>
-      </c>
-      <c r="N24" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B25" t="s">
-        <v>169</v>
-      </c>
-      <c r="C25" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" t="s">
-        <v>231</v>
-      </c>
-      <c r="F25" t="s">
-        <v>232</v>
-      </c>
-      <c r="G25" t="s">
-        <v>233</v>
-      </c>
-      <c r="K25">
-        <v>228366006</v>
-      </c>
-      <c r="L25" t="s">
-        <v>234</v>
-      </c>
-      <c r="M25" t="s">
-        <v>221</v>
-      </c>
-      <c r="N25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B26" t="s">
-        <v>169</v>
-      </c>
-      <c r="C26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>235</v>
-      </c>
-      <c r="F26" t="s">
-        <v>236</v>
-      </c>
-      <c r="G26" t="s">
-        <v>237</v>
-      </c>
-      <c r="K26">
-        <v>36456004</v>
-      </c>
-      <c r="L26" t="s">
-        <v>238</v>
-      </c>
-      <c r="M26" t="s">
-        <v>239</v>
-      </c>
-      <c r="N26" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B27" t="s">
-        <v>169</v>
-      </c>
-      <c r="C27" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
-        <v>241</v>
-      </c>
-      <c r="F27" t="s">
-        <v>242</v>
-      </c>
-      <c r="G27" t="s">
-        <v>242</v>
-      </c>
-      <c r="K27">
-        <v>36456004</v>
-      </c>
-      <c r="L27" t="s">
-        <v>238</v>
-      </c>
-      <c r="M27" t="s">
-        <v>239</v>
-      </c>
-      <c r="N27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="A28" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B28" t="s">
-        <v>169</v>
-      </c>
-      <c r="C28" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" t="s">
-        <v>112</v>
-      </c>
-      <c r="E28" t="s">
-        <v>243</v>
-      </c>
-      <c r="F28" t="s">
-        <v>244</v>
-      </c>
-      <c r="G28" t="s">
-        <v>244</v>
-      </c>
-      <c r="K28">
-        <v>36456004</v>
-      </c>
-      <c r="L28" t="s">
-        <v>238</v>
-      </c>
-      <c r="M28" t="s">
-        <v>239</v>
-      </c>
-      <c r="N28" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B29" t="s">
-        <v>169</v>
-      </c>
-      <c r="C29" t="s">
-        <v>170</v>
-      </c>
-      <c r="D29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" t="s">
-        <v>245</v>
-      </c>
-      <c r="F29" t="s">
-        <v>246</v>
-      </c>
-      <c r="G29" t="s">
-        <v>247</v>
-      </c>
-      <c r="I29" t="s">
-        <v>248</v>
-      </c>
-      <c r="J29" t="s">
-        <v>249</v>
-      </c>
-      <c r="M29" t="s">
-        <v>239</v>
-      </c>
-      <c r="N29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" t="s">
-        <v>170</v>
-      </c>
-      <c r="D30" t="s">
-        <v>112</v>
-      </c>
-      <c r="E30" t="s">
-        <v>250</v>
-      </c>
-      <c r="F30" t="s">
-        <v>251</v>
-      </c>
-      <c r="G30" t="s">
-        <v>252</v>
-      </c>
-      <c r="H30" t="s">
-        <v>253</v>
-      </c>
-      <c r="I30" t="s">
-        <v>153</v>
-      </c>
-      <c r="J30" t="s">
-        <v>154</v>
-      </c>
-      <c r="O30" t="s">
-        <v>254</v>
-      </c>
-      <c r="P30" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31" s="4">
-        <v>11223344</v>
-      </c>
-      <c r="B31" t="s">
-        <v>169</v>
-      </c>
-      <c r="C31" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" t="s">
-        <v>112</v>
-      </c>
-      <c r="E31" t="s">
-        <v>257</v>
-      </c>
-      <c r="F31" t="s">
-        <v>258</v>
-      </c>
-      <c r="G31" t="s">
-        <v>258</v>
-      </c>
-      <c r="H31" t="s">
-        <v>253</v>
-      </c>
-      <c r="I31" t="s">
-        <v>153</v>
-      </c>
-      <c r="J31" t="s">
-        <v>154</v>
-      </c>
-      <c r="M31" t="s">
-        <v>142</v>
-      </c>
-      <c r="N31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6C365E-EF48-4ACD-93DF-A89DE3724212}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4143,43 +3001,43 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>259</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>260</v>
+        <v>95</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>261</v>
+        <v>96</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>262</v>
+        <v>97</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>263</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>264</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>265</v>
+        <v>100</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>266</v>
+        <v>101</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>267</v>
+        <v>102</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>268</v>
+        <v>103</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>269</v>
+        <v>104</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>270</v>
+        <v>105</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>271</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.5">
@@ -4187,19 +3045,19 @@
         <v>11223344</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>274</v>
+        <v>109</v>
       </c>
       <c r="E2">
         <v>405672008</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>110</v>
       </c>
       <c r="G2" s="19" t="s">
         <v>55</v>
@@ -4214,16 +3072,16 @@
         <v>70</v>
       </c>
       <c r="K2" t="s">
-        <v>276</v>
+        <v>111</v>
       </c>
       <c r="L2" t="s">
-        <v>277</v>
+        <v>112</v>
       </c>
       <c r="M2" t="s">
         <v>70</v>
       </c>
       <c r="N2" t="s">
-        <v>278</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -4235,12 +3093,1253 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFCE62ED-6F52-49FE-89FA-F3C6891E8BA9}">
+  <dimension ref="A1:R31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="127.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="196" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" customWidth="1"/>
+    <col min="12" max="12" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="46.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="2" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" t="s">
+        <v>135</v>
+      </c>
+      <c r="J2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K2" t="s">
+        <v>137</v>
+      </c>
+      <c r="N2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N3" t="s">
+        <v>145</v>
+      </c>
+      <c r="O3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" t="s">
+        <v>149</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" t="s">
+        <v>151</v>
+      </c>
+      <c r="N4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K5" t="s">
+        <v>151</v>
+      </c>
+      <c r="N5" t="s">
+        <v>152</v>
+      </c>
+      <c r="O5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" t="s">
+        <v>132</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N6" t="s">
+        <v>162</v>
+      </c>
+      <c r="O6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" t="s">
+        <v>167</v>
+      </c>
+      <c r="K7" t="s">
+        <v>168</v>
+      </c>
+      <c r="N7" t="s">
+        <v>162</v>
+      </c>
+      <c r="O7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H8" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" t="s">
+        <v>172</v>
+      </c>
+      <c r="J8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K8" t="s">
+        <v>174</v>
+      </c>
+      <c r="N8" t="s">
+        <v>175</v>
+      </c>
+      <c r="O8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H9" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" t="s">
+        <v>172</v>
+      </c>
+      <c r="J9" t="s">
+        <v>173</v>
+      </c>
+      <c r="K9" t="s">
+        <v>174</v>
+      </c>
+      <c r="N9" t="s">
+        <v>175</v>
+      </c>
+      <c r="O9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="G10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" t="s">
+        <v>172</v>
+      </c>
+      <c r="J10" t="s">
+        <v>173</v>
+      </c>
+      <c r="K10" t="s">
+        <v>174</v>
+      </c>
+      <c r="N10" t="s">
+        <v>175</v>
+      </c>
+      <c r="O10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" t="s">
+        <v>184</v>
+      </c>
+      <c r="H11" t="s">
+        <v>185</v>
+      </c>
+      <c r="I11" t="s">
+        <v>172</v>
+      </c>
+      <c r="J11" t="s">
+        <v>173</v>
+      </c>
+      <c r="K11" t="s">
+        <v>174</v>
+      </c>
+      <c r="N11" t="s">
+        <v>175</v>
+      </c>
+      <c r="O11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="G12" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" t="s">
+        <v>188</v>
+      </c>
+      <c r="I12" t="s">
+        <v>172</v>
+      </c>
+      <c r="J12" t="s">
+        <v>173</v>
+      </c>
+      <c r="K12" t="s">
+        <v>174</v>
+      </c>
+      <c r="O12" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D13" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" t="s">
+        <v>193</v>
+      </c>
+      <c r="J13" t="s">
+        <v>194</v>
+      </c>
+      <c r="K13" t="s">
+        <v>195</v>
+      </c>
+      <c r="N13" t="s">
+        <v>196</v>
+      </c>
+      <c r="O13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" t="s">
+        <v>190</v>
+      </c>
+      <c r="E14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" t="s">
+        <v>199</v>
+      </c>
+      <c r="H14" t="s">
+        <v>200</v>
+      </c>
+      <c r="J14" t="s">
+        <v>201</v>
+      </c>
+      <c r="K14" t="s">
+        <v>202</v>
+      </c>
+      <c r="N14" t="s">
+        <v>203</v>
+      </c>
+      <c r="O14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" t="s">
+        <v>132</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="G15" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" t="s">
+        <v>207</v>
+      </c>
+      <c r="J15" t="s">
+        <v>208</v>
+      </c>
+      <c r="K15" t="s">
+        <v>209</v>
+      </c>
+      <c r="N15" t="s">
+        <v>210</v>
+      </c>
+      <c r="O15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" t="s">
+        <v>213</v>
+      </c>
+      <c r="H16" t="s">
+        <v>214</v>
+      </c>
+      <c r="J16" t="s">
+        <v>208</v>
+      </c>
+      <c r="K16" t="s">
+        <v>209</v>
+      </c>
+      <c r="N16" t="s">
+        <v>175</v>
+      </c>
+      <c r="O16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D17" t="s">
+        <v>190</v>
+      </c>
+      <c r="E17" t="s">
+        <v>132</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="G17" t="s">
+        <v>216</v>
+      </c>
+      <c r="H17" t="s">
+        <v>217</v>
+      </c>
+      <c r="L17">
+        <v>106133000</v>
+      </c>
+      <c r="M17" t="s">
+        <v>218</v>
+      </c>
+      <c r="N17" t="s">
+        <v>219</v>
+      </c>
+      <c r="O17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="G18" t="s">
+        <v>222</v>
+      </c>
+      <c r="H18" t="s">
+        <v>223</v>
+      </c>
+      <c r="L18">
+        <v>365458002</v>
+      </c>
+      <c r="M18" t="s">
+        <v>224</v>
+      </c>
+      <c r="N18" t="s">
+        <v>219</v>
+      </c>
+      <c r="O18" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G19" t="s">
+        <v>226</v>
+      </c>
+      <c r="H19" t="s">
+        <v>227</v>
+      </c>
+      <c r="L19">
+        <v>129861002</v>
+      </c>
+      <c r="M19" t="s">
+        <v>228</v>
+      </c>
+      <c r="N19" t="s">
+        <v>229</v>
+      </c>
+      <c r="O19" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B20" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" t="s">
+        <v>231</v>
+      </c>
+      <c r="H20" t="s">
+        <v>232</v>
+      </c>
+      <c r="L20">
+        <v>129861002</v>
+      </c>
+      <c r="M20" t="s">
+        <v>228</v>
+      </c>
+      <c r="N20" t="s">
+        <v>233</v>
+      </c>
+      <c r="O20" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E21" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="G21" t="s">
+        <v>235</v>
+      </c>
+      <c r="H21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22">
+        <v>228273003</v>
+      </c>
+      <c r="M22" t="s">
+        <v>240</v>
+      </c>
+      <c r="N22" t="s">
+        <v>241</v>
+      </c>
+      <c r="O22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B23" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="G23" t="s">
+        <v>244</v>
+      </c>
+      <c r="H23" t="s">
+        <v>245</v>
+      </c>
+      <c r="L23">
+        <v>365980008</v>
+      </c>
+      <c r="M23" t="s">
+        <v>246</v>
+      </c>
+      <c r="N23" t="s">
+        <v>241</v>
+      </c>
+      <c r="O23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="G24" t="s">
+        <v>248</v>
+      </c>
+      <c r="H24" t="s">
+        <v>249</v>
+      </c>
+      <c r="L24">
+        <v>409069009</v>
+      </c>
+      <c r="M24" t="s">
+        <v>250</v>
+      </c>
+      <c r="N24" t="s">
+        <v>241</v>
+      </c>
+      <c r="O24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B25" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D25" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="G25" t="s">
+        <v>252</v>
+      </c>
+      <c r="H25" t="s">
+        <v>253</v>
+      </c>
+      <c r="L25">
+        <v>228366006</v>
+      </c>
+      <c r="M25" t="s">
+        <v>254</v>
+      </c>
+      <c r="N25" t="s">
+        <v>241</v>
+      </c>
+      <c r="O25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="G26" t="s">
+        <v>256</v>
+      </c>
+      <c r="H26" t="s">
+        <v>257</v>
+      </c>
+      <c r="L26">
+        <v>36456004</v>
+      </c>
+      <c r="M26" t="s">
+        <v>258</v>
+      </c>
+      <c r="N26" t="s">
+        <v>259</v>
+      </c>
+      <c r="O26" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="G27" t="s">
+        <v>262</v>
+      </c>
+      <c r="H27" t="s">
+        <v>262</v>
+      </c>
+      <c r="L27">
+        <v>36456004</v>
+      </c>
+      <c r="M27" t="s">
+        <v>258</v>
+      </c>
+      <c r="N27" t="s">
+        <v>259</v>
+      </c>
+      <c r="O27" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" t="s">
+        <v>190</v>
+      </c>
+      <c r="E28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="G28" t="s">
+        <v>264</v>
+      </c>
+      <c r="H28" t="s">
+        <v>264</v>
+      </c>
+      <c r="L28">
+        <v>36456004</v>
+      </c>
+      <c r="M28" t="s">
+        <v>258</v>
+      </c>
+      <c r="N28" t="s">
+        <v>259</v>
+      </c>
+      <c r="O28" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D29" t="s">
+        <v>190</v>
+      </c>
+      <c r="E29" t="s">
+        <v>132</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="G29" t="s">
+        <v>266</v>
+      </c>
+      <c r="H29" t="s">
+        <v>267</v>
+      </c>
+      <c r="J29" t="s">
+        <v>268</v>
+      </c>
+      <c r="K29" t="s">
+        <v>269</v>
+      </c>
+      <c r="N29" t="s">
+        <v>259</v>
+      </c>
+      <c r="O29" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="G30" t="s">
+        <v>271</v>
+      </c>
+      <c r="H30" t="s">
+        <v>272</v>
+      </c>
+      <c r="I30" t="s">
+        <v>273</v>
+      </c>
+      <c r="J30" t="s">
+        <v>173</v>
+      </c>
+      <c r="K30" t="s">
+        <v>174</v>
+      </c>
+      <c r="P30" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>275</v>
+      </c>
+      <c r="R30" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="4">
+        <v>11223344</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" t="s">
+        <v>190</v>
+      </c>
+      <c r="E31" t="s">
+        <v>132</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="G31" t="s">
+        <v>278</v>
+      </c>
+      <c r="H31" t="s">
+        <v>278</v>
+      </c>
+      <c r="I31" t="s">
+        <v>273</v>
+      </c>
+      <c r="J31" t="s">
+        <v>173</v>
+      </c>
+      <c r="K31" t="s">
+        <v>174</v>
+      </c>
+      <c r="N31" t="s">
+        <v>162</v>
+      </c>
+      <c r="O31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D60A84-5E08-43D0-B361-C2827226B37C}">
-  <dimension ref="A1:N96"/>
+  <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97:XFD98"/>
+    <sheetView topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4256,22 +4355,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="13" customFormat="1" ht="15.75">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" s="14" customFormat="1" ht="15.75">
       <c r="A2" s="14" t="s">
@@ -4683,23 +4782,23 @@
         <v>298</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="8" customFormat="1">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:8" s="16" customFormat="1">
+      <c r="A21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="16" t="s">
         <v>289</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="F21" s="8" t="b">
+      <c r="F21" s="16" t="b">
         <v>1</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="16" t="s">
         <v>296</v>
       </c>
     </row>
@@ -4891,7 +4990,7 @@
       <c r="G30" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H30" s="23"/>
+      <c r="H30" s="24"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
@@ -4915,7 +5014,7 @@
       <c r="G31" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H31" s="23"/>
+      <c r="H31" s="24"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
@@ -4939,7 +5038,7 @@
       <c r="G32" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H32" s="23"/>
+      <c r="H32" s="24"/>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
@@ -4963,7 +5062,7 @@
       <c r="G33" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H33" s="23"/>
+      <c r="H33" s="24"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
@@ -4987,7 +5086,7 @@
       <c r="G34" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H34" s="23"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
@@ -5011,7 +5110,7 @@
       <c r="G35" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="H35" s="23"/>
+      <c r="H35" s="24"/>
     </row>
     <row r="36" spans="1:8" s="8" customFormat="1">
       <c r="A36" s="8" t="s">
@@ -5560,27 +5659,27 @@
       </c>
     </row>
     <row r="63" spans="1:7" s="8" customFormat="1">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64" spans="1:7" s="12" customFormat="1">
-      <c r="A64" s="21"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
     </row>
     <row r="65" spans="1:7" s="12" customFormat="1">
-      <c r="A65" s="21"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
+      <c r="A65" s="22"/>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1">
       <c r="A66" s="8" t="s">
@@ -5624,13 +5723,13 @@
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1">
       <c r="A68" s="8" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>323</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>302</v>
@@ -5644,13 +5743,13 @@
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1">
       <c r="A69" s="8" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B69" s="8" t="s">
         <v>323</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>302</v>
@@ -5664,13 +5763,13 @@
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1">
       <c r="A70" s="8" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B70" s="8" t="s">
         <v>323</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>302</v>
@@ -5684,13 +5783,13 @@
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1">
       <c r="A71" s="8" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B71" s="8" t="s">
         <v>323</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>302</v>
@@ -5704,13 +5803,13 @@
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1">
       <c r="A72" s="8" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>323</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>302</v>
@@ -5722,35 +5821,35 @@
         <v>296</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>100</v>
-      </c>
-      <c r="B73" t="s">
+    <row r="73" spans="1:7" s="8" customFormat="1">
+      <c r="A73" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D73" t="s">
-        <v>100</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="D73" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E73" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="F73" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>298</v>
+      <c r="F73" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
         <v>323</v>
       </c>
       <c r="D74" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E74" t="s">
         <v>302</v>
@@ -5764,13 +5863,13 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
         <v>323</v>
       </c>
       <c r="D75" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="E75" t="s">
         <v>302</v>
@@ -5784,13 +5883,13 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
         <v>323</v>
       </c>
       <c r="D76" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="E76" t="s">
         <v>302</v>
@@ -5804,13 +5903,13 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
         <v>323</v>
       </c>
       <c r="D77" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="E77" t="s">
         <v>302</v>
@@ -5824,13 +5923,13 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
         <v>323</v>
       </c>
       <c r="D78" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E78" t="s">
         <v>302</v>
@@ -5844,13 +5943,13 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B79" t="s">
         <v>323</v>
       </c>
       <c r="D79" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="E79" t="s">
         <v>302</v>
@@ -5864,13 +5963,13 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B80" t="s">
         <v>323</v>
       </c>
       <c r="D80" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="E80" t="s">
         <v>302</v>
@@ -5884,13 +5983,13 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B81" t="s">
         <v>323</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="E81" t="s">
         <v>302</v>
@@ -5904,13 +6003,13 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B82" t="s">
         <v>323</v>
       </c>
       <c r="D82" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="E82" t="s">
         <v>302</v>
@@ -5922,35 +6021,35 @@
         <v>298</v>
       </c>
     </row>
-    <row r="83" spans="1:7" s="8" customFormat="1">
-      <c r="A83" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="D83" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E83" s="8" t="s">
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>129</v>
+      </c>
+      <c r="B83" t="s">
+        <v>323</v>
+      </c>
+      <c r="D83" t="s">
+        <v>129</v>
+      </c>
+      <c r="E83" t="s">
         <v>302</v>
       </c>
-      <c r="F83" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G83" s="8" t="s">
-        <v>296</v>
+      <c r="F83" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" s="16" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="8" customFormat="1">
       <c r="A84" s="8" t="s">
-        <v>259</v>
+        <v>0</v>
       </c>
       <c r="B84" s="8" t="s">
         <v>324</v>
       </c>
       <c r="D84" s="8" t="s">
-        <v>259</v>
+        <v>0</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>302</v>
@@ -5964,13 +6063,13 @@
     </row>
     <row r="85" spans="1:7" s="8" customFormat="1">
       <c r="A85" s="8" t="s">
-        <v>260</v>
+        <v>94</v>
       </c>
       <c r="B85" s="8" t="s">
         <v>324</v>
       </c>
       <c r="D85" s="8" t="s">
-        <v>260</v>
+        <v>94</v>
       </c>
       <c r="E85" s="8" t="s">
         <v>302</v>
@@ -5984,13 +6083,13 @@
     </row>
     <row r="86" spans="1:7" s="8" customFormat="1">
       <c r="A86" s="8" t="s">
-        <v>261</v>
+        <v>95</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>324</v>
       </c>
       <c r="D86" s="8" t="s">
-        <v>261</v>
+        <v>95</v>
       </c>
       <c r="E86" s="8" t="s">
         <v>302</v>
@@ -6002,35 +6101,35 @@
         <v>296</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>262</v>
-      </c>
-      <c r="B87" t="s">
-        <v>325</v>
-      </c>
-      <c r="D87" t="s">
-        <v>262</v>
-      </c>
-      <c r="E87" t="s">
+    <row r="87" spans="1:7" s="8" customFormat="1">
+      <c r="A87" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="F87" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G87" s="16" t="s">
-        <v>298</v>
+      <c r="F87" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>263</v>
+        <v>97</v>
       </c>
       <c r="B88" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D88" t="s">
-        <v>263</v>
+        <v>97</v>
       </c>
       <c r="E88" t="s">
         <v>302</v>
@@ -6044,13 +6143,13 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>264</v>
+        <v>98</v>
       </c>
       <c r="B89" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D89" t="s">
-        <v>264</v>
+        <v>98</v>
       </c>
       <c r="E89" t="s">
         <v>302</v>
@@ -6062,35 +6161,35 @@
         <v>298</v>
       </c>
     </row>
-    <row r="90" spans="1:7" s="8" customFormat="1">
-      <c r="A90" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E90" s="8" t="s">
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" t="s">
+        <v>324</v>
+      </c>
+      <c r="D90" t="s">
+        <v>99</v>
+      </c>
+      <c r="E90" t="s">
         <v>302</v>
       </c>
-      <c r="F90" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>296</v>
+      <c r="F90" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="16" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:7" s="8" customFormat="1">
       <c r="A91" s="8" t="s">
-        <v>266</v>
+        <v>100</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>266</v>
+        <v>100</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>302</v>
@@ -6104,13 +6203,13 @@
     </row>
     <row r="92" spans="1:7" s="8" customFormat="1">
       <c r="A92" s="8" t="s">
-        <v>267</v>
+        <v>101</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>267</v>
+        <v>101</v>
       </c>
       <c r="E92" s="8" t="s">
         <v>302</v>
@@ -6122,35 +6221,35 @@
         <v>296</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
-      <c r="A93" t="s">
-        <v>268</v>
-      </c>
-      <c r="B93" t="s">
-        <v>326</v>
-      </c>
-      <c r="D93" t="s">
-        <v>268</v>
-      </c>
-      <c r="E93" t="s">
+    <row r="93" spans="1:7" s="8" customFormat="1">
+      <c r="A93" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E93" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="F93" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93" s="16" t="s">
-        <v>298</v>
+      <c r="F93" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>269</v>
+        <v>103</v>
       </c>
       <c r="B94" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D94" t="s">
-        <v>269</v>
+        <v>103</v>
       </c>
       <c r="E94" t="s">
         <v>302</v>
@@ -6162,35 +6261,35 @@
         <v>298</v>
       </c>
     </row>
-    <row r="95" spans="1:7" s="8" customFormat="1">
-      <c r="A95" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="B95" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="E95" s="8" t="s">
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B95" t="s">
+        <v>324</v>
+      </c>
+      <c r="D95" t="s">
+        <v>104</v>
+      </c>
+      <c r="E95" t="s">
         <v>302</v>
       </c>
-      <c r="F95" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" s="8" t="s">
-        <v>296</v>
+      <c r="F95" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G95" s="16" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="8" customFormat="1">
       <c r="A96" s="8" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>270</v>
+        <v>106</v>
       </c>
       <c r="E96" s="8" t="s">
         <v>302</v>
@@ -6199,6 +6298,26 @@
         <v>1</v>
       </c>
       <c r="G96" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="8" customFormat="1">
+      <c r="A97" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E97" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="F97" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G97" s="8" t="s">
         <v>296</v>
       </c>
     </row>

</xml_diff>